<commit_message>
Test plan for savings planed.
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_savings_account.xlsx
+++ b/tests/A02_pixell_test_plan_savings_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Updated Assignments ISD\assignment_02\given_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\rrc_polytec\Term 2\Intermidate Software Development\project\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5394E5-D09B-4C82-AD73-79542EE783C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA130629-E298-42CC-90AA-373ED0A99549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -233,9 +233,6 @@
     <t>balance less than minimum balance</t>
   </si>
   <si>
-    <t>Student Name</t>
-  </si>
-  <si>
     <t>Attributes are set to parameter values.</t>
   </si>
   <si>
@@ -246,6 +243,42 @@
   </si>
   <si>
     <t>balance  equal to minimum balance</t>
+  </si>
+  <si>
+    <t>Om Patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
+    <t>account_number=2004, client_number=2904, balance=1000.0, date_created=date(2024, 10, 5), minimum_balance=50.0</t>
+  </si>
+  <si>
+    <t>account_number=2004, client_number=2904, balance=1000.0, date_created=date(2024, 10, 5), minimum_balance="invalid"</t>
+  </si>
+  <si>
+    <t>minimum balance is set to be 50.0</t>
+  </si>
+  <si>
+    <t>account_number=2004, client_number=2904, balance=100.0, date_created=date(2024, 10, 5), minimum_balance=50.0</t>
+  </si>
+  <si>
+    <t>account_number=2004, client_number=2904, balance=50.0, date_created=date(2024, 10, 5), minimum_balance=50.0</t>
+  </si>
+  <si>
+    <t>account_number=2004, client_number=2904, balance=49.99, date_created=date(2024, 10, 5), minimum_balance=50.0</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Service charge is 0.50</t>
+  </si>
+  <si>
+    <t>Service charge is 1.00</t>
+  </si>
+  <si>
+    <t>String :- Account Number: 2004 Client Number: 2904 Balance: $1,000.00 Minimum Balance: $50.00 Account Type: Savings</t>
   </si>
 </sst>
 </file>
@@ -1152,22 +1185,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="53.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1179,16 +1211,16 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1197,10 +1229,10 @@
       </c>
       <c r="D4" s="20"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1228,13 +1260,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1244,11 +1282,17 @@
       <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1256,13 +1300,19 @@
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1270,13 +1320,19 @@
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>5</v>
       </c>
@@ -1286,11 +1342,17 @@
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1298,13 +1360,19 @@
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1314,7 +1382,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>8</v>
       </c>
@@ -1324,7 +1392,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1334,7 +1402,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
         <v>10</v>
       </c>
@@ -1344,7 +1412,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -1354,7 +1422,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1364,7 +1432,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1374,7 +1442,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1384,7 +1452,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1394,7 +1462,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1404,7 +1472,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1414,7 +1482,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1424,7 +1492,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1434,7 +1502,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>20</v>
       </c>
@@ -1444,7 +1512,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1454,7 +1522,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
         <v>22</v>
       </c>
@@ -1464,7 +1532,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>23</v>
       </c>
@@ -1474,7 +1542,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1484,7 +1552,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="11">
         <v>25</v>
       </c>
@@ -1494,7 +1562,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
         <v>26</v>
       </c>
@@ -1504,7 +1572,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
         <v>6</v>
       </c>

</xml_diff>